<commit_message>
contact and vendor ut
abstracted test method, setup and tear down, fixed excel files to run
properly
</commit_message>
<xml_diff>
--- a/UT.Vend.BLL/HelperFiles/Contact.xlsx
+++ b/UT.Vend.BLL/HelperFiles/Contact.xlsx
@@ -11,24 +11,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>ContactID</t>
+  </si>
+  <si>
+    <t>ContactFirstName</t>
+  </si>
+  <si>
+    <t>ContactMiddleName</t>
+  </si>
+  <si>
+    <t>ContactLastName</t>
+  </si>
+  <si>
+    <t>ActiveFlg</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
   <si>
     <t>Volteer.Vend.tblContact</t>
-  </si>
-  <si>
-    <t>ContactID</t>
-  </si>
-  <si>
-    <t>ContactFirstName</t>
-  </si>
-  <si>
-    <t>ContactMiddleName</t>
-  </si>
-  <si>
-    <t>ContactLastName</t>
-  </si>
-  <si>
-    <t>ActiveFlag</t>
   </si>
   <si>
     <t>FFE96E44-6447-4AB6-8EFA-0F8604D479E6</t>
@@ -206,250 +212,282 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="42.29"/>
-    <col min="6" customWidth="1" max="6" width="37.29"/>
+    <col min="1" customWidth="1" max="1" width="21.71"/>
+    <col min="2" customWidth="1" max="2" width="42.29"/>
+    <col min="7" customWidth="1" max="7" width="186.43"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" r="A1">
         <v>0</v>
       </c>
+      <c t="s" r="B1">
+        <v>1</v>
+      </c>
+      <c t="s" r="C1">
+        <v>2</v>
+      </c>
+      <c t="s" r="D1">
+        <v>3</v>
+      </c>
+      <c t="s" r="E1">
+        <v>4</v>
+      </c>
+      <c t="s" r="F1">
+        <v>5</v>
+      </c>
+      <c t="s" r="G1">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c t="s" r="B2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c t="s" r="C2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c t="s" r="D2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c t="s" r="E2">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <f>RANDBETWEEN(0,1)</f>
+        <v>1</v>
+      </c>
+      <c t="str" r="G2">
+        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp;"')"</f>
+        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlg) VALUES('FFE96E44-6447-4AB6-8EFA-0F8604D479E6','Anthony','Kevin','Smith','1')</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c t="s" r="B3">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c t="s" r="C3">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c t="s" r="D3">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <f>RANDBETWEEN(0,1)</f>
-        <v>0</v>
-      </c>
-      <c t="str" r="F3">
-        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ",") &amp; $D$2) &amp; ",") &amp; $E$2) &amp; ") VALUES('") &amp; RC[-5]) &amp;"',") &amp; B3) &amp;"',") &amp; RC[-3]) &amp;"',") &amp; D3) &amp;"',") &amp; RC[-1]) &amp;"')"</f>
-        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlag) VALUES('FFE96E44-6447-4AB6-8EFA-0F8604D479E6',Anthony',Kevin',Smith',0')</v>
+        <v>14</v>
+      </c>
+      <c t="s" r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <f>RANDBETWEEN(0,1)</f>
+        <v>1</v>
+      </c>
+      <c t="str" r="G3">
+        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp;"')"</f>
+        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlg) VALUES('85C79F05-FF2D-46CB-8481-0FE71FD4B348','Bobby','Larry','Jones','1')</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c t="s" r="B4">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c t="s" r="C4">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c t="s" r="D4">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <f>RANDBETWEEN(0,1)</f>
-        <v>1</v>
-      </c>
-      <c t="str" r="F4">
-        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ",") &amp; $D$2) &amp; ",") &amp; $E$2) &amp; ") VALUES('") &amp; RC[-5]) &amp;"',") &amp; B4) &amp;"',") &amp; RC[-3]) &amp;"',") &amp; D4) &amp;"',") &amp; RC[-1]) &amp;"')"</f>
-        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlag) VALUES('85C79F05-FF2D-46CB-8481-0FE71FD4B348',Bobby',Larry',Jones',1')</v>
+        <v>18</v>
+      </c>
+      <c t="s" r="E4">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <f>RANDBETWEEN(0,1)</f>
+        <v>1</v>
+      </c>
+      <c t="str" r="G4">
+        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp;"')"</f>
+        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlg) VALUES('BBCF5EBB-7932-4BB0-AFAB-1445C0AEDB91','Carmen','Matt','Johnson','1')</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c t="s" r="B5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c t="s" r="C5">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c t="s" r="D5">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <f>RANDBETWEEN(0,1)</f>
-        <v>0</v>
-      </c>
-      <c t="str" r="F5">
-        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ",") &amp; $D$2) &amp; ",") &amp; $E$2) &amp; ") VALUES('") &amp; RC[-5]) &amp;"',") &amp; B5) &amp;"',") &amp; RC[-3]) &amp;"',") &amp; D5) &amp;"',") &amp; RC[-1]) &amp;"')"</f>
-        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlag) VALUES('BBCF5EBB-7932-4BB0-AFAB-1445C0AEDB91',Carmen',Matt',Johnson',0')</v>
+        <v>22</v>
+      </c>
+      <c t="s" r="E5">
+        <v>23</v>
+      </c>
+      <c r="F5">
+        <f>RANDBETWEEN(0,1)</f>
+        <v>1</v>
+      </c>
+      <c t="str" r="G5">
+        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp;"')"</f>
+        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlg) VALUES('055127D5-14B1-4843-B0F9-23E451FEDC11','Dennis','Nick','Williams','1')</v>
       </c>
     </row>
     <row r="6">
       <c t="s" r="A6">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c t="s" r="B6">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c t="s" r="C6">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c t="s" r="D6">
-        <v>21</v>
-      </c>
-      <c r="E6">
-        <f>RANDBETWEEN(0,1)</f>
-        <v>0</v>
-      </c>
-      <c t="str" r="F6">
-        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ",") &amp; $D$2) &amp; ",") &amp; $E$2) &amp; ") VALUES('") &amp; RC[-5]) &amp;"',") &amp; B6) &amp;"',") &amp; RC[-3]) &amp;"',") &amp; D6) &amp;"',") &amp; RC[-1]) &amp;"')"</f>
-        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlag) VALUES('055127D5-14B1-4843-B0F9-23E451FEDC11',Dennis',Nick',Williams',0')</v>
+        <v>26</v>
+      </c>
+      <c t="s" r="E6">
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <f>RANDBETWEEN(0,1)</f>
+        <v>1</v>
+      </c>
+      <c t="str" r="G6">
+        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp;"')"</f>
+        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlg) VALUES('5C05FE31-BF50-41BB-B5B3-3B67710DEC1A','Eric','Oliver','Brown','1')</v>
       </c>
     </row>
     <row r="7">
       <c t="s" r="A7">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c t="s" r="B7">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c t="s" r="C7">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c t="s" r="D7">
-        <v>25</v>
-      </c>
-      <c r="E7">
-        <f>RANDBETWEEN(0,1)</f>
-        <v>0</v>
-      </c>
-      <c t="str" r="F7">
-        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ",") &amp; $D$2) &amp; ",") &amp; $E$2) &amp; ") VALUES('") &amp; RC[-5]) &amp;"',") &amp; B7) &amp;"',") &amp; RC[-3]) &amp;"',") &amp; D7) &amp;"',") &amp; RC[-1]) &amp;"')"</f>
-        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlag) VALUES('5C05FE31-BF50-41BB-B5B3-3B67710DEC1A',Eric',Oliver',Brown',0')</v>
+        <v>30</v>
+      </c>
+      <c t="s" r="E7">
+        <v>31</v>
+      </c>
+      <c r="F7">
+        <f>RANDBETWEEN(0,1)</f>
+        <v>1</v>
+      </c>
+      <c t="str" r="G7">
+        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp;"')"</f>
+        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlg) VALUES('0FC01234-B8AA-4705-8FF9-4596D4AF8CFC','Frank','Patrick','Davis','1')</v>
       </c>
     </row>
     <row r="8">
       <c t="s" r="A8">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c t="s" r="B8">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c t="s" r="C8">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c t="s" r="D8">
-        <v>29</v>
-      </c>
-      <c r="E8">
+        <v>34</v>
+      </c>
+      <c t="s" r="E8">
+        <v>35</v>
+      </c>
+      <c r="F8">
         <f>RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
-      <c t="str" r="F8">
-        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ",") &amp; $D$2) &amp; ",") &amp; $E$2) &amp; ") VALUES('") &amp; RC[-5]) &amp;"',") &amp; B8) &amp;"',") &amp; RC[-3]) &amp;"',") &amp; D8) &amp;"',") &amp; RC[-1]) &amp;"')"</f>
-        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlag) VALUES('0FC01234-B8AA-4705-8FF9-4596D4AF8CFC',Frank',Patrick',Davis',0')</v>
+      <c t="str" r="G8">
+        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp;"')"</f>
+        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlg) VALUES('5A41B01E-7F59-4DD2-A6C4-4CAD882BC0AB','George','Que','Wilson','0')</v>
       </c>
     </row>
     <row r="9">
       <c t="s" r="A9">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c t="s" r="B9">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c t="s" r="C9">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c t="s" r="D9">
-        <v>33</v>
-      </c>
-      <c r="E9">
-        <f>RANDBETWEEN(0,1)</f>
-        <v>1</v>
-      </c>
-      <c t="str" r="F9">
-        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ",") &amp; $D$2) &amp; ",") &amp; $E$2) &amp; ") VALUES('") &amp; RC[-5]) &amp;"',") &amp; B9) &amp;"',") &amp; RC[-3]) &amp;"',") &amp; D9) &amp;"',") &amp; RC[-1]) &amp;"')"</f>
-        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlag) VALUES('5A41B01E-7F59-4DD2-A6C4-4CAD882BC0AB',George',Que',Wilson',1')</v>
+        <v>38</v>
+      </c>
+      <c t="s" r="E9">
+        <v>39</v>
+      </c>
+      <c r="F9">
+        <f>RANDBETWEEN(0,1)</f>
+        <v>0</v>
+      </c>
+      <c t="str" r="G9">
+        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp;"')"</f>
+        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlg) VALUES('B6702B43-223D-48B3-88FF-6E463A521261','Harry','Robert','Moore','0')</v>
       </c>
     </row>
     <row r="10">
       <c t="s" r="A10">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c t="s" r="B10">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c t="s" r="C10">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c t="s" r="D10">
-        <v>37</v>
-      </c>
-      <c r="E10">
-        <f>RANDBETWEEN(0,1)</f>
-        <v>1</v>
-      </c>
-      <c t="str" r="F10">
-        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ",") &amp; $D$2) &amp; ",") &amp; $E$2) &amp; ") VALUES('") &amp; RC[-5]) &amp;"',") &amp; B10) &amp;"',") &amp; RC[-3]) &amp;"',") &amp; D10) &amp;"',") &amp; RC[-1]) &amp;"')"</f>
-        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlag) VALUES('B6702B43-223D-48B3-88FF-6E463A521261',Harry',Robert',Moore',1')</v>
+        <v>42</v>
+      </c>
+      <c t="s" r="E10">
+        <v>43</v>
+      </c>
+      <c r="F10">
+        <f>RANDBETWEEN(0,1)</f>
+        <v>0</v>
+      </c>
+      <c t="str" r="G10">
+        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp;"')"</f>
+        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlg) VALUES('E4922B15-BA01-49C5-A541-A73A2EC461D9','Ian','Steve','Anderson','0')</v>
       </c>
     </row>
     <row r="11">
       <c t="s" r="A11">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c t="s" r="B11">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c t="s" r="C11">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c t="s" r="D11">
-        <v>41</v>
-      </c>
-      <c r="E11">
-        <f>RANDBETWEEN(0,1)</f>
-        <v>0</v>
-      </c>
-      <c t="str" r="F11">
-        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ",") &amp; $D$2) &amp; ",") &amp; $E$2) &amp; ") VALUES('") &amp; RC[-5]) &amp;"',") &amp; B11) &amp;"',") &amp; RC[-3]) &amp;"',") &amp; D11) &amp;"',") &amp; RC[-1]) &amp;"')"</f>
-        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlag) VALUES('E4922B15-BA01-49C5-A541-A73A2EC461D9',Ian',Steve',Anderson',0')</v>
-      </c>
-    </row>
-    <row r="12">
-      <c t="s" r="A12">
-        <v>42</v>
-      </c>
-      <c t="s" r="B12">
-        <v>43</v>
-      </c>
-      <c t="s" r="C12">
-        <v>44</v>
-      </c>
-      <c t="s" r="D12">
-        <v>45</v>
-      </c>
-      <c r="E12">
-        <f>RANDBETWEEN(0,1)</f>
-        <v>0</v>
-      </c>
-      <c t="str" r="F12">
-        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$1) &amp;" (") &amp; $A$2) &amp; ",") &amp; $B$2) &amp; ",") &amp; $C$2) &amp; ",") &amp; $D$2) &amp; ",") &amp; $E$2) &amp; ") VALUES('") &amp; RC[-5]) &amp;"',") &amp; B12) &amp;"',") &amp; RC[-3]) &amp;"',") &amp; D12) &amp;"',") &amp; RC[-1]) &amp;"')"</f>
-        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlag) VALUES('1222663B-C1D4-4593-A288-AADC1AF70E70',Justin',Thomas',Taylor',0')</v>
+        <v>46</v>
+      </c>
+      <c t="s" r="E11">
+        <v>47</v>
+      </c>
+      <c r="F11">
+        <f>RANDBETWEEN(0,1)</f>
+        <v>1</v>
+      </c>
+      <c t="str" r="G11">
+        <f>((((((((((((((((((((("INSERT INTO " &amp; $A$2) &amp;" (") &amp; $B$1) &amp; ",") &amp; $C$1) &amp; ",") &amp; $D$1) &amp; ",") &amp; $E$1) &amp; ",") &amp; $F$1) &amp; ") VALUES('") &amp; RC[-5]) &amp;"','") &amp; RC[-4]) &amp;"','") &amp; RC[-3]) &amp;"','") &amp; RC[-2]) &amp;"','") &amp; RC[-1]) &amp;"')"</f>
+        <v>INSERT INTO Volteer.Vend.tblContact (ContactID,ContactFirstName,ContactMiddleName,ContactLastName,ActiveFlg) VALUES('1222663B-C1D4-4593-A288-AADC1AF70E70','Justin','Thomas','Taylor','1')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>